<commit_message>
partial saturation in geotechnical materials lib
</commit_message>
<xml_diff>
--- a/m500 Geotechnical Examples/500 Geotechnical Material Library.xlsx
+++ b/m500 Geotechnical Examples/500 Geotechnical Material Library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\repos\LusasNoteBooks\m500 Geotechnical Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB08894-C5C9-483D-A363-D6DD233BA0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB06FD9-BA25-4948-9CDC-E7B75CCDA472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A42CF2A5-1928-46F0-BE98-8406D117E106}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Elastic</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Two phase</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -469,43 +472,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="6">
     <dxf>
       <font>
         <strike/>
@@ -563,83 +559,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -975,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C8989F-2427-4FB0-8200-EDD712EDED77}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,7 +938,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1039,7 +958,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1057,7 +976,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1075,7 +994,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="32" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1095,7 +1014,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="25" t="s">
         <v>14</v>
       </c>
@@ -1113,7 +1032,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="25" t="s">
         <v>20</v>
       </c>
@@ -1132,7 +1051,7 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="25" t="s">
         <v>26</v>
       </c>
@@ -1151,7 +1070,7 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="25" t="s">
         <v>53</v>
       </c>
@@ -1170,7 +1089,7 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="25" t="s">
         <v>23</v>
       </c>
@@ -1189,7 +1108,7 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="8" t="s">
         <v>25</v>
       </c>
@@ -1208,189 +1127,189 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="28">
         <v>2100</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="28">
         <v>2100</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="28">
         <v>2100</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="1">
         <v>0.4</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="1">
         <v>0.3</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="1">
         <v>0.2</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="1">
         <f>0.5/60/60/24</f>
         <v>5.7870370370370367E-6</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15" s="1">
         <f>1/60/60/24</f>
         <v>1.1574074074074073E-5</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="1">
         <f>1/60/60/24</f>
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="1">
         <f t="shared" ref="D16:D17" si="0">0.5/60/60/24</f>
         <v>5.7870370370370367E-6</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="1">
         <f t="shared" ref="E16:F17" si="1">1/60/60/24</f>
         <v>1.1574074074074073E-5</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="1">
         <f t="shared" si="1"/>
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36" t="s">
+      <c r="A17" s="34"/>
+      <c r="B17" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="37">
+      <c r="D17" s="1">
         <f t="shared" si="0"/>
         <v>5.7870370370370367E-6</v>
       </c>
-      <c r="E17" s="37">
+      <c r="E17" s="1">
         <f t="shared" si="1"/>
         <v>1.1574074074074073E-5</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="1">
         <f t="shared" si="1"/>
         <v>1.1574074074074073E-5</v>
       </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="36" t="s">
+      <c r="A18" s="34"/>
+      <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="1">
         <v>1</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36" t="s">
+      <c r="A19" s="34"/>
+      <c r="B19" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="38" t="s">
-        <v>57</v>
-      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36" t="s">
+      <c r="A20" s="34"/>
+      <c r="B20" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="E20" s="37">
+      <c r="E20" s="1">
         <v>0</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F20" s="1">
         <v>0</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
-      <c r="B21" s="36" t="s">
+      <c r="A21" s="34"/>
+      <c r="B21" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="37">
+      <c r="E21" s="1">
         <v>1</v>
       </c>
-      <c r="F21" s="37">
+      <c r="F21" s="1">
         <v>1</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="13" t="s">
         <v>40</v>
       </c>
@@ -1456,34 +1375,34 @@
     <mergeCell ref="A6:A12"/>
     <mergeCell ref="A13:A22"/>
   </mergeCells>
+  <conditionalFormatting sqref="D11:D12">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$D$10="No cut-off"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D20:D22">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$D$19="Fully"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E12">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$E$10="No cut-off"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>$E$19="Fully"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F22">
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>$F$19="Fully"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F11:F12">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$F$10="No cut-off"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D12">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$D$10="No cut-off"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E12">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$E$10="No cut-off"</formula>
+  <conditionalFormatting sqref="F20:F22">
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>$F$19="Fully"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -1491,7 +1410,7 @@
       <formula1>"No cut-off, Rankine, Pressure"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19:F19" xr:uid="{D09CF0EC-4027-4AEC-9D86-60207C3D72A5}">
-      <formula1>"Fully,Partially"</formula1>
+      <formula1>"Fully,Partially,None"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>